<commit_message>
Activate 3 system simulations
</commit_message>
<xml_diff>
--- a/src/data/Queue Advanced.xlsx
+++ b/src/data/Queue Advanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Folder\College\Simulation and Modelling\simulation-project\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C35990-9F55-4889-8948-2F4513F11D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA9FE57-D2A2-47F4-B7A9-53781A811372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,15 +1232,15 @@
       </c>
       <c r="F15" s="4">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="G15" s="4">
         <f ca="1">LOOKUP(F15,$J$4:$K$9,$G$4:$G$9)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15" s="4">
         <f ca="1">E15+G15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="4">
         <f>E15-D15</f>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="K15" s="4">
         <f ca="1">H15-D15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1259,32 +1259,32 @@
         <v>2</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" ref="B16:B24" ca="1" si="6">RANDBETWEEN(1,1000)</f>
-        <v>691</v>
+        <f t="shared" ref="B16:B34" ca="1" si="6">RANDBETWEEN(1,1000)</f>
+        <v>949</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" ref="C16:C24" ca="1" si="7">LOOKUP(B16,$D$4:$E$11,$A$4:$A$11)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16" s="4">
         <f ca="1">C16+D15</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4">
         <f ca="1">MAX(D16,H15)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16:F24" ca="1" si="8">RANDBETWEEN(1,100)</f>
-        <v>1</v>
+        <f t="shared" ref="F16:F34" ca="1" si="8">RANDBETWEEN(1,100)</f>
+        <v>64</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" ref="G16:G24" ca="1" si="9">LOOKUP(F16,$J$4:$K$9,$G$4:$G$9)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" ref="H16:H24" ca="1" si="10">E16+G16</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" ref="I16:I24" ca="1" si="11">E16-D16</f>
@@ -1292,11 +1292,11 @@
       </c>
       <c r="J16" s="4">
         <f ca="1">E16-H15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" ref="K16:K24" ca="1" si="12">H16-D16</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1305,31 +1305,31 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>131</v>
+        <v>808</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" ref="D17:D24" ca="1" si="13">C17+D16</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" ref="E17:E24" ca="1" si="14">MAX(D17,H16)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" ca="1" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" ca="1" si="11"/>
@@ -1337,11 +1337,11 @@
       </c>
       <c r="J17" s="4">
         <f t="shared" ref="J17:J24" ca="1" si="15">E17-H16</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K17" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1350,23 +1350,23 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>251</v>
+        <v>665</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" ca="1" si="9"/>
@@ -1374,19 +1374,19 @@
       </c>
       <c r="H18" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K18" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1395,23 +1395,23 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>459</v>
+        <v>662</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" ca="1" si="9"/>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="H19" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" ca="1" si="11"/>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="J19" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K19" s="4">
         <f t="shared" ca="1" si="12"/>
@@ -1440,23 +1440,23 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>236</v>
+        <v>935</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" ca="1" si="9"/>
@@ -1464,19 +1464,19 @@
       </c>
       <c r="H20" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1485,31 +1485,31 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>740</v>
+        <v>856</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" ca="1" si="11"/>
@@ -1517,11 +1517,11 @@
       </c>
       <c r="J21" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1530,43 +1530,43 @@
       </c>
       <c r="B22" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>229</v>
+        <v>673</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="F22" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K22" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M22" s="2"/>
     </row>
@@ -1576,31 +1576,31 @@
       </c>
       <c r="B23" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>905</v>
+        <v>807</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" ca="1" si="11"/>
@@ -1608,11 +1608,11 @@
       </c>
       <c r="J23" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K23" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M23" s="2"/>
     </row>
@@ -1622,31 +1622,31 @@
       </c>
       <c r="B24" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>361</v>
+        <v>541</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" ca="1" si="14"/>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" ca="1" si="8"/>
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" ca="1" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" ca="1" si="10"/>
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="I24" s="4">
         <f t="shared" ca="1" si="11"/>
@@ -1654,51 +1654,401 @@
       </c>
       <c r="J24" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" ca="1" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>11</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>955</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" ref="C25:C34" ca="1" si="16">LOOKUP(B25,$D$4:$E$11,$A$4:$A$11)</f>
+        <v>8</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" ref="D25:D34" ca="1" si="17">C25+D24</f>
+        <v>68</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" ref="E25:E34" ca="1" si="18">MAX(D25,H24)</f>
+        <v>68</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>27</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" ref="G25:G34" ca="1" si="19">LOOKUP(F25,$J$4:$K$9,$G$4:$G$9)</f>
+        <v>2</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" ref="H25:H34" ca="1" si="20">E25+G25</f>
+        <v>70</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" ref="I25:I34" ca="1" si="21">E25-D25</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" ref="J25:J34" ca="1" si="22">E25-H24</f>
+        <v>5</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" ref="K25:K34" ca="1" si="23">H25-D25</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>12</v>
+      </c>
+      <c r="B26" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>817</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>75</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>75</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>76</v>
+      </c>
+      <c r="I26" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>452</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" ca="1" si="16"/>
         <v>4</v>
       </c>
-      <c r="M24" s="2"/>
+      <c r="D27" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>79</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>79</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>81</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>14</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>79</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>80</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>81</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>93</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>5</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>86</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>6</v>
+      </c>
       <c r="M28" s="7" t="s">
         <v>18</v>
       </c>
       <c r="N28" s="3">
         <f ca="1">SUM(I15:I24)/10</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>15</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>669</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>86</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>86</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>76</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>90</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>4</v>
+      </c>
       <c r="M29" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N29" s="3">
         <f ca="1">COUNTIF(I15:I24, "&gt;0") / 10</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>16</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>88</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>90</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>73</v>
+      </c>
+      <c r="G30" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>94</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>6</v>
+      </c>
       <c r="M30" s="7" t="s">
         <v>20</v>
       </c>
       <c r="N30" s="3">
         <f ca="1">SUM(J15:J24)/(E15+H24)</f>
-        <v>0.32500000000000001</v>
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>17</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>508</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>93</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>94</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>97</v>
+      </c>
+      <c r="I31" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>4</v>
+      </c>
       <c r="M31" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N31" s="3">
         <f ca="1">SUM(G15:G24)/10</f>
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>18</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>563</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>98</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>98</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>100</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>2</v>
+      </c>
       <c r="M32" s="7" t="s">
         <v>22</v>
       </c>
@@ -1707,31 +2057,117 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="33" spans="13:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>19</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>95</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>99</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>100</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>59</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>103</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>4</v>
+      </c>
       <c r="M33" s="7" t="s">
         <v>23</v>
       </c>
       <c r="N33" s="3">
         <f ca="1">SUM(C15:C24)/9</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>20</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" ca="1" si="6"/>
+        <v>900</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" ca="1" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" ca="1" si="17"/>
+        <v>107</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" ca="1" si="18"/>
+        <v>107</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" ca="1" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>108</v>
+      </c>
+      <c r="I34" s="4">
+        <f t="shared" ca="1" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="4">
+        <f t="shared" ca="1" si="22"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="13:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="K34" s="4">
+        <f t="shared" ca="1" si="23"/>
+        <v>1</v>
+      </c>
       <c r="M34" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="3" t="e">
         <f ca="1">SUM(I15:I24) / COUNTIF(I15:I24,"&gt;0")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="13:14" ht="18.75" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="M35" s="7" t="s">
         <v>25</v>
       </c>
       <c r="N35" s="3">
         <f ca="1">SUM(K15:K24)/10</f>
-        <v>3</v>
+        <v>3.3</v>
       </c>
     </row>
   </sheetData>
@@ -1741,7 +2177,7 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="J15:J24">
+  <conditionalFormatting sqref="J15:J34">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>